<commit_message>
09/05/2016 Nouvelle palette (IGN)
Signed-off-by: loyak64 <loyak64@hotmail.fr>
</commit_message>
<xml_diff>
--- a/Convertisseur_couleurs_RGB.xlsx
+++ b/Convertisseur_couleurs_RGB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Couleurs RGB 0 à 255</t>
   </si>
@@ -52,13 +52,76 @@
   </si>
   <si>
     <t>#132960</t>
+  </si>
+  <si>
+    <t>Palette 20 couleurs</t>
+  </si>
+  <si>
+    <t>#003366</t>
+  </si>
+  <si>
+    <t>#164B67</t>
+  </si>
+  <si>
+    <t>#2B6368</t>
+  </si>
+  <si>
+    <t>#417C69</t>
+  </si>
+  <si>
+    <t>#57946A</t>
+  </si>
+  <si>
+    <t>#6CAC6B</t>
+  </si>
+  <si>
+    <t>#82C46C</t>
+  </si>
+  <si>
+    <t>#9BCE72</t>
+  </si>
+  <si>
+    <t>#B4D779</t>
+  </si>
+  <si>
+    <t>#CDFE17</t>
+  </si>
+  <si>
+    <t>#E6EA86</t>
+  </si>
+  <si>
+    <t>#FFF48D</t>
+  </si>
+  <si>
+    <t>#E7D878</t>
+  </si>
+  <si>
+    <t>#CFBB64</t>
+  </si>
+  <si>
+    <t>#B79D50</t>
+  </si>
+  <si>
+    <t>#A0803C</t>
+  </si>
+  <si>
+    <t>#886328</t>
+  </si>
+  <si>
+    <t>#704614</t>
+  </si>
+  <si>
+    <t>#582900</t>
+  </si>
+  <si>
+    <t>#000000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +153,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -150,11 +219,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,6 +323,53 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -475,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -488,7 +685,7 @@
     <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -504,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -526,7 +723,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="4">
         <v>19</v>
       </c>
@@ -553,7 +750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="4">
         <v>35</v>
       </c>
@@ -580,7 +777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="4">
         <v>69</v>
       </c>
@@ -607,7 +804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="4">
         <v>77</v>
       </c>
@@ -634,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:11" ht="15.75">
       <c r="A7" s="4">
         <v>65</v>
       </c>
@@ -661,176 +858,171 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75">
+    <row r="8" spans="1:11" ht="15.75">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75">
+      <c r="A9" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
       <c r="E11" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75">
+        <v>0.4</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="23"/>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
       <c r="E12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75">
+        <v>0.41</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
       <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75">
+        <v>0.41</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
       <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75">
+        <v>0.42</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
       <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75">
+        <v>0.42</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
       <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="3"/>
+        <v>0.42</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="4"/>
@@ -838,18 +1030,17 @@
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="3"/>
+        <v>0.45</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="4"/>
@@ -857,18 +1048,17 @@
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
       <c r="E18" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.71</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="G18" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="3"/>
+        <v>0.47</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="15.75">
       <c r="A19" s="4"/>
@@ -876,18 +1066,17 @@
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
       <c r="E19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="4"/>
@@ -895,18 +1084,17 @@
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
       <c r="E20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F20" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.92</v>
       </c>
       <c r="G20" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="3"/>
+        <v>0.53</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="4"/>
@@ -914,18 +1102,17 @@
       <c r="C21" s="6"/>
       <c r="D21" s="3"/>
       <c r="E21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.96</v>
       </c>
       <c r="G21" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="3"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="4"/>
@@ -933,18 +1120,17 @@
       <c r="C22" s="6"/>
       <c r="D22" s="3"/>
       <c r="E22" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="G22" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="3"/>
+        <v>0.47</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="4"/>
@@ -952,18 +1138,17 @@
       <c r="C23" s="6"/>
       <c r="D23" s="3"/>
       <c r="E23" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="F23" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="G23" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="3"/>
+        <v>0.39</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="15.75">
       <c r="A24" s="4"/>
@@ -971,18 +1156,17 @@
       <c r="C24" s="6"/>
       <c r="D24" s="3"/>
       <c r="E24" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.72</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="G24" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="3"/>
+        <v>0.31</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="15.75">
       <c r="A25" s="4"/>
@@ -990,18 +1174,17 @@
       <c r="C25" s="6"/>
       <c r="D25" s="3"/>
       <c r="E25" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G25" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="3"/>
+        <v>0.24</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="15.75">
       <c r="A26" s="4"/>
@@ -1009,18 +1192,17 @@
       <c r="C26" s="6"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="G26" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="3"/>
+        <v>0.16</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="15.75">
       <c r="A27" s="4"/>
@@ -1028,18 +1210,17 @@
       <c r="C27" s="6"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="F27" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G27" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="15.75">
       <c r="A28" s="4"/>
@@ -1047,18 +1228,17 @@
       <c r="C28" s="6"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="F28" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="G28" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="15.75">
       <c r="A29" s="4"/>
@@ -1066,18 +1246,17 @@
       <c r="C29" s="6"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F29" s="5">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="15.75">
       <c r="A30" s="4"/>
@@ -1085,15 +1264,12 @@
       <c r="C30" s="6"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F30" s="5">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G30" s="6">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I30" s="3"/>
@@ -1104,15 +1280,12 @@
       <c r="C31" s="6"/>
       <c r="D31" s="3"/>
       <c r="E31" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G31" s="6">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I31" s="3"/>
@@ -1123,23 +1296,22 @@
       <c r="C32" s="6"/>
       <c r="D32" s="3"/>
       <c r="E32" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F32" s="5">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G32" s="6">
-        <f>ROUND(C32/255,2)</f>
         <v>0</v>
       </c>
       <c r="I32" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="A9:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>